<commit_message>
add Headless mode for Chrome
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="42">
   <si>
     <t>Keyword</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>TC # 01.01 - Shop by search and category</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Test</t>
+  </si>
+  <si>
+    <t>TC # 01.01</t>
+  </si>
+  <si>
+    <t>TC # 01.02</t>
   </si>
 </sst>
 </file>
@@ -558,15 +567,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="8" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
@@ -600,7 +609,9 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -611,7 +622,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
@@ -626,7 +639,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
@@ -639,7 +654,9 @@
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
@@ -654,7 +671,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
@@ -669,7 +688,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
@@ -684,7 +705,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
@@ -697,7 +720,9 @@
       <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
@@ -712,7 +737,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B11" s="6" t="s">
         <v>3</v>
       </c>
@@ -727,7 +754,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
@@ -740,7 +769,9 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B13" s="6" t="s">
         <v>32</v>
       </c>
@@ -755,7 +786,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B14" s="6" t="s">
         <v>8</v>
       </c>
@@ -768,7 +801,9 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B15" s="6" t="s">
         <v>8</v>
       </c>
@@ -781,7 +816,9 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B16" s="6" t="s">
         <v>8</v>
       </c>
@@ -794,7 +831,9 @@
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
@@ -807,7 +846,9 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
@@ -820,7 +861,9 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B19" s="6" t="s">
         <v>32</v>
       </c>
@@ -835,7 +878,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B20" s="6" t="s">
         <v>8</v>
       </c>
@@ -848,7 +893,9 @@
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B21" s="6" t="s">
         <v>8</v>
       </c>
@@ -861,7 +908,9 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B22" s="6" t="s">
         <v>19</v>
       </c>
@@ -876,7 +925,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B23" s="6" t="s">
         <v>19</v>
       </c>
@@ -898,6 +949,357 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="11"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add api DP, appManager refactoring
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="o7032SJrUYCbjSJahVa3tHyKW+30Fnh6DC85aAcYgdh8Oohh1wj3TS/m/K+54l9Pqh4/DIa1jFrTT5wQGsAjgQ==" workbookSaltValue="Cvg/1FRpudUyBYKAzd/OfQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="9288" tabRatio="331"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10872" windowHeight="4968" tabRatio="331"/>
   </bookViews>
   <sheets>
     <sheet name="UItests" sheetId="1" r:id="rId1"/>
+    <sheet name="APItests" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -101,46 +101,46 @@
     <t>volchanskij@gmail.com</t>
   </si>
   <si>
+    <t>My account - My Store</t>
+  </si>
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>Printed Summer Dress</t>
+  </si>
+  <si>
+    <t>SELECTITEM</t>
+  </si>
+  <si>
+    <t>addToCartButton</t>
+  </si>
+  <si>
+    <t>closeOverlayButton</t>
+  </si>
+  <si>
+    <t>proceedToCheckoutButton</t>
+  </si>
+  <si>
+    <t>Printed Dress</t>
+  </si>
+  <si>
+    <t>homeButton</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Shop by search and category</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Test</t>
+  </si>
+  <si>
+    <t>TC # 01.01</t>
+  </si>
+  <si>
+    <t>TC # 01.02</t>
+  </si>
+  <si>
     <t>testPWD001</t>
-  </si>
-  <si>
-    <t>My account - My Store</t>
-  </si>
-  <si>
-    <t>items</t>
-  </si>
-  <si>
-    <t>Printed Summer Dress</t>
-  </si>
-  <si>
-    <t>SELECTITEM</t>
-  </si>
-  <si>
-    <t>addToCartButton</t>
-  </si>
-  <si>
-    <t>closeOverlayButton</t>
-  </si>
-  <si>
-    <t>proceedToCheckoutButton</t>
-  </si>
-  <si>
-    <t>Printed Dress</t>
-  </si>
-  <si>
-    <t>homeButton</t>
-  </si>
-  <si>
-    <t>TC # 01.01 - Shop by search and category</t>
-  </si>
-  <si>
-    <t>TC # 01.02 - Test</t>
-  </si>
-  <si>
-    <t>TC # 01.01</t>
-  </si>
-  <si>
-    <t>TC # 01.02</t>
   </si>
 </sst>
 </file>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,7 +601,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
@@ -610,7 +610,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>4</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>14</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>14</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>3</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>3</v>
@@ -701,12 +701,12 @@
         <v>12</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>8</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>14</v>
@@ -733,12 +733,12 @@
         <v>12</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>3</v>
@@ -750,12 +750,12 @@
         <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>8</v>
@@ -770,30 +770,30 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
@@ -802,13 +802,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -817,13 +817,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>12</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>8</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>8</v>
@@ -862,30 +862,30 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
@@ -894,13 +894,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>12</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>19</v>
@@ -921,12 +921,12 @@
         <v>12</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>19</v>
@@ -938,7 +938,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -952,7 +952,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
@@ -961,7 +961,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>4</v>
@@ -974,7 +974,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>14</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>8</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>14</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>3</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>3</v>
@@ -1052,12 +1052,12 @@
         <v>12</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>8</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>14</v>
@@ -1084,12 +1084,12 @@
         <v>12</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>3</v>
@@ -1101,12 +1101,12 @@
         <v>12</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>8</v>
@@ -1121,30 +1121,30 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>12</v>
@@ -1153,13 +1153,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>12</v>
@@ -1168,13 +1168,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>12</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>8</v>
@@ -1198,7 +1198,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>8</v>
@@ -1213,30 +1213,30 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>12</v>
@@ -1245,13 +1245,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>12</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>19</v>
@@ -1272,12 +1272,12 @@
         <v>12</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>19</v>
@@ -1289,7 +1289,7 @@
         <v>12</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1305,4 +1305,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Hero Image Validation TC, add VERIFYSLIDER action to  UIOperation.class, refactor of UIOperation.class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="UItests" sheetId="1" r:id="rId1"/>
-    <sheet name="APItests" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="68">
   <si>
     <t>Keyword</t>
   </si>
@@ -26,21 +25,12 @@
     <t>value</t>
   </si>
   <si>
-    <t>SETTEXT</t>
-  </si>
-  <si>
     <t>GOTOURL</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>ObjectType</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>CLICK</t>
   </si>
   <si>
@@ -56,12 +46,6 @@
     <t>css</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>VERIFYTITLE</t>
-  </si>
-  <si>
     <t>shopLoginButton</t>
   </si>
   <si>
@@ -110,9 +94,6 @@
     <t>Printed Summer Dress</t>
   </si>
   <si>
-    <t>SELECTITEM</t>
-  </si>
-  <si>
     <t>addToCartButton</t>
   </si>
   <si>
@@ -131,9 +112,6 @@
     <t>TC # 01.01 - Shop by search and category</t>
   </si>
   <si>
-    <t>TC # 01.02 - Test</t>
-  </si>
-  <si>
     <t>TC # 01.01</t>
   </si>
   <si>
@@ -141,13 +119,112 @@
   </si>
   <si>
     <t>testPWD001</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Sign Up</t>
+  </si>
+  <si>
+    <t>createAccountButton</t>
+  </si>
+  <si>
+    <t>genderRadioButton</t>
+  </si>
+  <si>
+    <t>firstNameTextField</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>lastNameTextField</t>
+  </si>
+  <si>
+    <t>bruno</t>
+  </si>
+  <si>
+    <t>newPasswordTextField</t>
+  </si>
+  <si>
+    <t>newAddressTextField</t>
+  </si>
+  <si>
+    <t>178 somwhere I belong</t>
+  </si>
+  <si>
+    <t>newCityTextField</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>stateDropDownMenu</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>newPostCodeTextField</t>
+  </si>
+  <si>
+    <t>newMobilePhoneTextField</t>
+  </si>
+  <si>
+    <t>registerAccountButton</t>
+  </si>
+  <si>
+    <t>CHOOSEFROM</t>
+  </si>
+  <si>
+    <t>94108</t>
+  </si>
+  <si>
+    <t>4158695625</t>
+  </si>
+  <si>
+    <t>CLICKRADIOBUTTON</t>
+  </si>
+  <si>
+    <t>actualTitle</t>
+  </si>
+  <si>
+    <t>SETTEXTIN</t>
+  </si>
+  <si>
+    <t>VERIFYPAGETITLE</t>
+  </si>
+  <si>
+    <t>usernameField</t>
+  </si>
+  <si>
+    <t>passwordField</t>
+  </si>
+  <si>
+    <t>newUserNameField</t>
+  </si>
+  <si>
+    <t>SETUNIQUETEXTIN</t>
+  </si>
+  <si>
+    <t>SELECPAGETITEMFROM</t>
+  </si>
+  <si>
+    <t>TC # 01.03 - Hero Image Verification</t>
+  </si>
+  <si>
+    <t>VERIFYSLIDER</t>
+  </si>
+  <si>
+    <t>homeSlider</t>
+  </si>
+  <si>
+    <t>TC # 01.03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +270,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2F2F2F"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -249,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -259,9 +342,12 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -567,16 +653,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="8" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="34.88671875" customWidth="1"/>
@@ -584,7 +670,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -593,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -601,7 +687,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
@@ -610,711 +696,723 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="9" t="s">
-        <v>23</v>
+      <c r="E3" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>26</v>
+        <v>9</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>5</v>
+        <v>57</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>41</v>
+        <v>9</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>28</v>
+        <v>9</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="10"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="9" t="s">
-        <v>23</v>
+      <c r="E26" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>26</v>
+        <v>9</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>5</v>
+        <v>62</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="E31" s="11"/>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="E32" s="14"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>13</v>
+        <v>57</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>28</v>
+        <v>9</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>29</v>
+        <v>57</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>33</v>
+        <v>52</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>21</v>
+        <v>57</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="6" t="s">
+      <c r="A43" s="1"/>
+      <c r="B43" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="13"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="1"/>
+      <c r="A44" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>35</v>
+        <v>3</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="B46" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-      <c r="B47" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add SORTBY case using AsyncJS
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="67">
   <si>
     <t>Keyword</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>My Store</t>
-  </si>
-  <si>
-    <t>link</t>
   </si>
   <si>
     <t>Login - My Store</t>
@@ -655,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,7 +684,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
@@ -696,7 +693,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -709,13 +706,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -726,7 +723,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>5</v>
@@ -735,64 +732,64 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>5</v>
@@ -807,27 +804,27 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
@@ -836,12 +833,12 @@
         <v>9</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>5</v>
@@ -856,30 +853,30 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
@@ -888,13 +885,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
@@ -903,13 +900,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -918,7 +915,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>5</v>
@@ -933,7 +930,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>5</v>
@@ -948,30 +945,30 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
@@ -980,13 +977,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
@@ -995,7 +992,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>14</v>
@@ -1007,12 +1004,12 @@
         <v>9</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>14</v>
@@ -1024,7 +1021,7 @@
         <v>9</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1038,7 +1035,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
@@ -1047,7 +1044,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>3</v>
@@ -1060,13 +1057,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>9</v>
@@ -1077,7 +1074,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>5</v>
@@ -1086,53 +1083,53 @@
         <v>6</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>9</v>
@@ -1141,13 +1138,13 @@
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>9</v>
@@ -1156,149 +1153,149 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>9</v>
@@ -1307,19 +1304,19 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1333,7 +1330,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="2"/>
@@ -1342,7 +1339,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>3</v>
@@ -1355,13 +1352,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>9</v>
@@ -1372,13 +1369,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>9</v>
@@ -1387,13 +1384,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
add VERIFYLOWESTPRICEFIRST case based on Regex, Refactoring of UIOperation
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -85,9 +85,6 @@
     <t>My account - My Store</t>
   </si>
   <si>
-    <t>items</t>
-  </si>
-  <si>
     <t>Printed Summer Dress</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>TC # 01.03</t>
+  </si>
+  <si>
+    <t>itemName</t>
   </si>
 </sst>
 </file>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,7 +684,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
@@ -693,7 +693,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -706,13 +706,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>5</v>
@@ -738,13 +738,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
@@ -755,13 +755,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
@@ -772,24 +772,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>5</v>
@@ -804,13 +804,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
@@ -821,10 +821,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
@@ -833,12 +833,12 @@
         <v>9</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>5</v>
@@ -853,30 +853,30 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
@@ -885,13 +885,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
@@ -900,13 +900,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>5</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>5</v>
@@ -945,30 +945,30 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
@@ -977,13 +977,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>14</v>
@@ -1004,12 +1004,12 @@
         <v>9</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>14</v>
@@ -1021,7 +1021,7 @@
         <v>9</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1035,7 +1035,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>3</v>
@@ -1057,13 +1057,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>9</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>5</v>
@@ -1089,13 +1089,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>9</v>
@@ -1106,13 +1106,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>9</v>
@@ -1123,13 +1123,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>9</v>
@@ -1138,13 +1138,13 @@
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>9</v>
@@ -1153,149 +1153,149 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C38" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>9</v>
@@ -1304,13 +1304,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>9</v>
@@ -1330,7 +1330,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="2"/>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>3</v>
@@ -1352,13 +1352,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>9</v>
@@ -1369,13 +1369,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>9</v>
@@ -1384,13 +1384,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
regex functionality refactoring, add SETMAXPRICE
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="81">
   <si>
     <t>Keyword</t>
   </si>
@@ -220,9 +220,6 @@
     <t>TC # 01.04 - Use Sort by Price (Low to High)</t>
   </si>
   <si>
-    <t>http://automationpractice.com/index.php?id_category=3&amp;controller=category</t>
-  </si>
-  <si>
     <t>Women - My Store</t>
   </si>
   <si>
@@ -251,6 +248,15 @@
   </si>
   <si>
     <t>TC # 01.04</t>
+  </si>
+  <si>
+    <t>VERIFYBROKENIMAGES</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>womenSection</t>
   </si>
 </sst>
 </file>
@@ -686,16 +692,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" style="8" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="34.88671875" customWidth="1"/>
@@ -762,10 +768,10 @@
         <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
@@ -777,48 +783,46 @@
         <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>20</v>
-      </c>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -828,14 +832,14 @@
       <c r="B9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>58</v>
+      <c r="C9" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -843,89 +847,89 @@
         <v>30</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="12"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
@@ -942,7 +946,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -954,15 +958,17 @@
         <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -972,7 +978,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
@@ -987,10 +993,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E19" s="12"/>
     </row>
@@ -1002,10 +1008,10 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E20" s="12"/>
     </row>
@@ -1014,17 +1020,15 @@
         <v>30</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>27</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1034,10 +1038,10 @@
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E22" s="12"/>
     </row>
@@ -1046,143 +1050,141 @@
         <v>30</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="12"/>
+      <c r="E23" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>27</v>
-      </c>
+      <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="E25" s="12"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="5"/>
+      <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="12"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="11" t="s">
-        <v>18</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="B30" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="11"/>
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1190,95 +1192,95 @@
         <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="10"/>
+      <c r="E33" s="12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>59</v>
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="E35" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E36" s="14"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>36</v>
+        <v>78</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>39</v>
+      <c r="E38" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1286,34 +1288,30 @@
         <v>31</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>41</v>
+        <v>53</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="E40" s="14"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -1323,13 +1321,13 @@
         <v>55</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="10" t="s">
-        <v>44</v>
+      <c r="E41" s="12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1337,16 +1335,16 @@
         <v>31</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1357,13 +1355,13 @@
         <v>55</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1374,13 +1372,13 @@
         <v>55</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1388,31 +1386,33 @@
         <v>31</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="10"/>
+      <c r="E45" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1420,145 +1420,163 @@
         <v>31</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>77</v>
+        <v>55</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="10"/>
+      <c r="E47" s="10" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="13"/>
+      <c r="A48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="5"/>
+      <c r="A49" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="11" t="s">
-        <v>18</v>
+        <v>56</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="13"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="12"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-      <c r="B55" s="7" t="s">
-        <v>8</v>
+      <c r="B55" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="13"/>
+      <c r="E55" s="11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
+      <c r="A56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="11" t="s">
-        <v>68</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="10"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>56</v>
@@ -1570,18 +1588,18 @@
         <v>9</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B59" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>9</v>
@@ -1590,13 +1608,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="C60" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>9</v>
@@ -1604,45 +1622,153 @@
       <c r="E60" s="12"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>73</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="13"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="12"/>
+      <c r="A62" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-      <c r="B63" s="7" t="s">
-        <v>8</v>
+      <c r="A63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="13"/>
+      <c r="E63" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="12"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="12"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="12"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="12"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add posivite and err handl tests, add maven options
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10875" windowHeight="4965" tabRatio="331"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10872" windowHeight="4968" tabRatio="331" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="UItests" sheetId="1" r:id="rId1"/>
+    <sheet name="Positive" sheetId="1" r:id="rId1"/>
+    <sheet name="ErrorHandling" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="95">
   <si>
     <t>Keyword</t>
   </si>
@@ -278,12 +279,33 @@
   </si>
   <si>
     <t>TC # 01.05 - Use slider for setting price range (Max)</t>
+  </si>
+  <si>
+    <t>TC # 01.06 - Search can`t find results</t>
+  </si>
+  <si>
+    <t>TC # 01.06</t>
+  </si>
+  <si>
+    <t>~!@#$%^&amp;*()_+</t>
+  </si>
+  <si>
+    <t>Search - My Store</t>
+  </si>
+  <si>
+    <t>VERIFYSEARCHRESULTS</t>
+  </si>
+  <si>
+    <t>searchError</t>
+  </si>
+  <si>
+    <t>No results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -715,20 +737,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -745,7 +767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -754,7 +776,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -767,7 +789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -784,7 +806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -799,7 +821,7 @@
       </c>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -814,7 +836,7 @@
       </c>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -829,7 +851,7 @@
       </c>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -846,7 +868,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -863,7 +885,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -880,7 +902,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -895,7 +917,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -912,7 +934,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -927,7 +949,7 @@
       </c>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -942,7 +964,7 @@
       </c>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -959,7 +981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -974,7 +996,7 @@
       </c>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -991,7 +1013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1006,7 +1028,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1021,7 +1043,7 @@
       </c>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1036,7 +1058,7 @@
       </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1051,7 +1073,7 @@
       </c>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -1066,7 +1088,7 @@
       </c>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1083,7 +1105,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1098,7 +1120,7 @@
       </c>
       <c r="E24" s="12"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -1113,7 +1135,7 @@
       </c>
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -1130,7 +1152,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -1147,7 +1169,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1162,7 +1184,7 @@
       </c>
       <c r="E28" s="12"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1177,7 +1199,7 @@
       </c>
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="7" t="s">
         <v>8</v>
@@ -1186,7 +1208,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -1195,7 +1217,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1208,7 +1230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1225,7 +1247,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1240,7 +1262,7 @@
       </c>
       <c r="E34" s="11"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -1257,7 +1279,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>31</v>
       </c>
@@ -1272,7 +1294,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
@@ -1287,7 +1309,7 @@
       </c>
       <c r="E37" s="10"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
@@ -1304,7 +1326,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
@@ -1319,7 +1341,7 @@
       </c>
       <c r="E39" s="11"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
@@ -1334,7 +1356,7 @@
       </c>
       <c r="E40" s="14"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
@@ -1351,7 +1373,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>31</v>
       </c>
@@ -1368,7 +1390,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>31</v>
       </c>
@@ -1385,7 +1407,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>31</v>
       </c>
@@ -1402,7 +1424,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>31</v>
       </c>
@@ -1419,7 +1441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>31</v>
       </c>
@@ -1436,7 +1458,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>31</v>
       </c>
@@ -1453,7 +1475,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
@@ -1470,7 +1492,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>31</v>
       </c>
@@ -1485,7 +1507,7 @@
       </c>
       <c r="E49" s="10"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>31</v>
       </c>
@@ -1502,7 +1524,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>31</v>
       </c>
@@ -1517,7 +1539,7 @@
       </c>
       <c r="E51" s="10"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>31</v>
       </c>
@@ -1532,7 +1554,7 @@
       </c>
       <c r="E52" s="10"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="7" t="s">
         <v>8</v>
@@ -1541,7 +1563,7 @@
       <c r="D53" s="1"/>
       <c r="E53" s="13"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>62</v>
       </c>
@@ -1550,7 +1572,7 @@
       <c r="D54" s="2"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>65</v>
       </c>
@@ -1563,7 +1585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>65</v>
       </c>
@@ -1580,7 +1602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>65</v>
       </c>
@@ -1595,7 +1617,7 @@
       </c>
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -1612,7 +1634,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
@@ -1627,7 +1649,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>65</v>
       </c>
@@ -1642,7 +1664,7 @@
       </c>
       <c r="E60" s="12"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="7" t="s">
         <v>8</v>
@@ -1651,7 +1673,7 @@
       <c r="D61" s="1"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>67</v>
       </c>
@@ -1660,7 +1682,7 @@
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>77</v>
       </c>
@@ -1673,7 +1695,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>77</v>
       </c>
@@ -1688,7 +1710,7 @@
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
@@ -1705,7 +1727,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>77</v>
       </c>
@@ -1720,7 +1742,7 @@
       </c>
       <c r="E66" s="12"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>77</v>
       </c>
@@ -1735,7 +1757,7 @@
       </c>
       <c r="E67" s="12"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>77</v>
       </c>
@@ -1750,7 +1772,7 @@
       </c>
       <c r="E68" s="12"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>77</v>
       </c>
@@ -1767,7 +1789,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>77</v>
       </c>
@@ -1782,7 +1804,7 @@
       </c>
       <c r="E70" s="12"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="7" t="s">
         <v>8</v>
@@ -1791,7 +1813,7 @@
       <c r="D71" s="1"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>87</v>
       </c>
@@ -1800,7 +1822,7 @@
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>86</v>
       </c>
@@ -1813,7 +1835,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>86</v>
       </c>
@@ -1828,7 +1850,7 @@
       </c>
       <c r="E74" s="12"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>86</v>
       </c>
@@ -1845,7 +1867,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>86</v>
       </c>
@@ -1860,7 +1882,7 @@
       </c>
       <c r="E76" s="12"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>86</v>
       </c>
@@ -1875,7 +1897,7 @@
       </c>
       <c r="E77" s="12"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>86</v>
       </c>
@@ -1890,7 +1912,7 @@
       </c>
       <c r="E78" s="12"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>86</v>
       </c>
@@ -1905,7 +1927,7 @@
       </c>
       <c r="E79" s="12"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>86</v>
       </c>
@@ -1920,7 +1942,7 @@
       </c>
       <c r="E80" s="12"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="7" t="s">
         <v>8</v>
@@ -1933,4 +1955,190 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="35.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="13"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix SureFire report TC naming, finish refactoring stage 1
</commit_message>
<xml_diff>
--- a/src/test/resources/TestCase.xlsx
+++ b/src/test/resources/TestCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10875" windowHeight="4965" tabRatio="331" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10872" windowHeight="4968" tabRatio="331"/>
   </bookViews>
   <sheets>
     <sheet name="Positive" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="254">
   <si>
     <t>Keyword</t>
   </si>
@@ -107,12 +107,6 @@
     <t>TC # 01.01 - Shop by search and category</t>
   </si>
   <si>
-    <t>TC # 01.01</t>
-  </si>
-  <si>
-    <t>TC # 01.02</t>
-  </si>
-  <si>
     <t>testPWD001</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>homeSlider</t>
   </si>
   <si>
-    <t>TC # 01.03</t>
-  </si>
-  <si>
     <t>itemName</t>
   </si>
   <si>
@@ -248,9 +239,6 @@
     <t>weblinks</t>
   </si>
   <si>
-    <t>TC # 01.04</t>
-  </si>
-  <si>
     <t>VERIFYBROKENIMAGES</t>
   </si>
   <si>
@@ -275,9 +263,6 @@
     <t>VERIFYPRICERANGE(MAX)</t>
   </si>
   <si>
-    <t>TC # 01.05</t>
-  </si>
-  <si>
     <t>TC # 01.05 - Use slider for setting price range (Max)</t>
   </si>
   <si>
@@ -299,9 +284,6 @@
     <t>TC # 02.01 - Search can`t find results</t>
   </si>
   <si>
-    <t>TC # 02.01</t>
-  </si>
-  <si>
     <t>@gmail.com</t>
   </si>
   <si>
@@ -350,25 +332,457 @@
     <t>TC # 02.02 - Handling Error During Sign Up</t>
   </si>
   <si>
-    <t>TC # 02.02</t>
-  </si>
-  <si>
     <t>TC # 02.03 - Handling Error when filling personal information (Create An Account)</t>
   </si>
   <si>
-    <t>TC # 02.03</t>
-  </si>
-  <si>
     <t>TC # 02.04 - Handling Error During Log In</t>
   </si>
   <si>
-    <t>TC # 02.04</t>
+    <t>TC # 02.01 - Step 1</t>
+  </si>
+  <si>
+    <t>TC # 02.01 - Step 2</t>
+  </si>
+  <si>
+    <t>TC # 02.01 - Step 3</t>
+  </si>
+  <si>
+    <t>TC # 02.01 - Step 4</t>
+  </si>
+  <si>
+    <t>TC # 02.01 - Step 5</t>
+  </si>
+  <si>
+    <t>TC # 02.01 - Step 6</t>
+  </si>
+  <si>
+    <t>TC # 02.01 - Step 7</t>
+  </si>
+  <si>
+    <t>TC # 02.01 - Step 8</t>
+  </si>
+  <si>
+    <t>TC # 02.01 - Step 9</t>
+  </si>
+  <si>
+    <t>TC # 02.02 - Step 1</t>
+  </si>
+  <si>
+    <t>TC # 02.02 - Step 2</t>
+  </si>
+  <si>
+    <t>TC # 02.02 - Step 3</t>
+  </si>
+  <si>
+    <t>TC # 02.02 - Step 4</t>
+  </si>
+  <si>
+    <t>TC # 02.02 - Step 5</t>
+  </si>
+  <si>
+    <t>TC # 02.02 - Step 6</t>
+  </si>
+  <si>
+    <t>TC # 02.02 - Step 7</t>
+  </si>
+  <si>
+    <t>TC # 02.02 - Step 8</t>
+  </si>
+  <si>
+    <t>TC # 02.02 - Step 9</t>
+  </si>
+  <si>
+    <t>TC # 02.02 - Step 10</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 1</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 2</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 3</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 4</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 5</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 6</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 7</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 8</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 9</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 10</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 11</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 12</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 13</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 14</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 15</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 16</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 17</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 18</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 19</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 20</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 21</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 22</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 23</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 24</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 25</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 26</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 27</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 28</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 29</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 30</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 31</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 32</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 33</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 34</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 35</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 36</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 37</t>
+  </si>
+  <si>
+    <t>TC # 02.03 - Step 38</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 1</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 2</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 3</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 4</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 5</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 6</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 7</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 8</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 9</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 10</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 11</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 12</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 13</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 14</t>
+  </si>
+  <si>
+    <t>TC # 02.04 - Step 15</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 1</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 2</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 3</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 4</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 5</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 6</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 7</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 8</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 9</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 10</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 11</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 12</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 13</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 14</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 15</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 16</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 17</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 18</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 19</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 20</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 21</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 22</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 23</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 24</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 25</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 26</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 27</t>
+  </si>
+  <si>
+    <t>TC # 01.01 - Step 28</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 1</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 2</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 3</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 4</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 5</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 6</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 7</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 8</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 9</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 10</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 11</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 12</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 13</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 14</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 15</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 16</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 17</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 18</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 19</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 20</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 21</t>
+  </si>
+  <si>
+    <t>TC # 01.02 - Step 22</t>
+  </si>
+  <si>
+    <t>TC # 01.03 - Step 1</t>
+  </si>
+  <si>
+    <t>TC # 01.03 - Step 2</t>
+  </si>
+  <si>
+    <t>TC # 01.03 - Step 3</t>
+  </si>
+  <si>
+    <t>TC # 01.03 - Step 4</t>
+  </si>
+  <si>
+    <t>TC # 01.03 - Step 5</t>
+  </si>
+  <si>
+    <t>TC # 01.03 - Step 6</t>
+  </si>
+  <si>
+    <t>TC # 01.03 - Step 7</t>
+  </si>
+  <si>
+    <t>TC # 01.04 - Step 1</t>
+  </si>
+  <si>
+    <t>TC # 01.04 - Step 2</t>
+  </si>
+  <si>
+    <t>TC # 01.04 - Step 3</t>
+  </si>
+  <si>
+    <t>TC # 01.04 - Step 4</t>
+  </si>
+  <si>
+    <t>TC # 01.04 - Step 5</t>
+  </si>
+  <si>
+    <t>TC # 01.04 - Step 6</t>
+  </si>
+  <si>
+    <t>TC # 01.04 - Step 7</t>
+  </si>
+  <si>
+    <t>TC # 01.04 - Step 8</t>
+  </si>
+  <si>
+    <t>TC # 01.04 - Step 9</t>
+  </si>
+  <si>
+    <t>TC # 01.05 - Step 1</t>
+  </si>
+  <si>
+    <t>TC # 01.05 - Step 2</t>
+  </si>
+  <si>
+    <t>TC # 01.05 - Step 3</t>
+  </si>
+  <si>
+    <t>TC # 01.05 - Step 4</t>
+  </si>
+  <si>
+    <t>TC # 01.05 - Step 5</t>
+  </si>
+  <si>
+    <t>TC # 01.05 - Step 6</t>
+  </si>
+  <si>
+    <t>TC # 01.05 - Step 7</t>
+  </si>
+  <si>
+    <t>TC # 01.05 - Step 8</t>
+  </si>
+  <si>
+    <t>TC # 01.05 - Step 9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -812,20 +1226,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -842,7 +1256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -851,9 +1265,9 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>179</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -864,15 +1278,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -881,39 +1295,39 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>181</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>183</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>5</v>
@@ -926,15 +1340,15 @@
       </c>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>184</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
@@ -943,15 +1357,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>185</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
@@ -960,26 +1374,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>187</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
@@ -992,15 +1406,15 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>188</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
@@ -1009,42 +1423,42 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
@@ -1056,9 +1470,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>192</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>5</v>
@@ -1071,15 +1485,15 @@
       </c>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>193</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
@@ -1088,9 +1502,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>194</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>5</v>
@@ -1103,9 +1517,9 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>195</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>5</v>
@@ -1118,9 +1532,9 @@
       </c>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>196</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>5</v>
@@ -1133,9 +1547,9 @@
       </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>197</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>5</v>
@@ -1148,9 +1562,9 @@
       </c>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>198</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>5</v>
@@ -1163,15 +1577,15 @@
       </c>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>199</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
@@ -1180,9 +1594,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>5</v>
@@ -1195,9 +1609,9 @@
       </c>
       <c r="E24" s="12"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>201</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>5</v>
@@ -1210,9 +1624,9 @@
       </c>
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>202</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>14</v>
@@ -1227,9 +1641,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>203</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>14</v>
@@ -1244,38 +1658,40 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>204</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="12"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>206</v>
+      </c>
       <c r="B30" s="7" t="s">
         <v>8</v>
       </c>
@@ -1283,18 +1699,18 @@
       <c r="D30" s="1"/>
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>207</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>3</v>
@@ -1305,15 +1721,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>208</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>9</v>
@@ -1322,9 +1738,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>31</v>
+        <v>209</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>5</v>
@@ -1337,15 +1753,15 @@
       </c>
       <c r="E34" s="11"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>9</v>
@@ -1354,45 +1770,45 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>31</v>
+        <v>211</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E37" s="10"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>31</v>
+        <v>213</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>9</v>
@@ -1401,196 +1817,196 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>31</v>
+        <v>214</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="11"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="14"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="11"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="6" t="s">
+      <c r="D41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="14"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="9" t="s">
+      <c r="C42" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="12" t="s">
+      <c r="D42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="9" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="10" t="s">
+      <c r="D43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="9" t="s">
+      <c r="D44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="9" t="s">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="10" t="s">
+      <c r="D45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="9" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="10" t="s">
+      <c r="D46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="6" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>31</v>
+        <v>224</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E49" s="10"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>31</v>
+        <v>225</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>9</v>
@@ -1599,38 +2015,40 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>31</v>
+        <v>226</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D52" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E52" s="10"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="B53" s="7" t="s">
         <v>8</v>
       </c>
@@ -1638,18 +2056,18 @@
       <c r="D53" s="1"/>
       <c r="E53" s="13"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>3</v>
@@ -1660,15 +2078,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>65</v>
+        <v>230</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>9</v>
@@ -1677,30 +2095,30 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>65</v>
+        <v>231</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>65</v>
+        <v>232</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>9</v>
@@ -1709,38 +2127,40 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>65</v>
+        <v>233</v>
       </c>
       <c r="B59" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="12"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="12"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D60" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E60" s="12"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="B61" s="7" t="s">
         <v>8</v>
       </c>
@@ -1748,18 +2168,18 @@
       <c r="D61" s="1"/>
       <c r="E61" s="13"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>77</v>
+        <v>236</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>3</v>
@@ -1770,117 +2190,119 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>77</v>
+        <v>237</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>77</v>
+        <v>238</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E65" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="12"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="12"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="12"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="12"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="12"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B68" s="6" t="s">
+      <c r="D69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C68" s="1" t="s">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="12"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="D70" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E70" s="12"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>244</v>
+      </c>
       <c r="B71" s="7" t="s">
         <v>8</v>
       </c>
@@ -1888,18 +2310,18 @@
       <c r="D71" s="1"/>
       <c r="E71" s="13"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>86</v>
+        <v>245</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>3</v>
@@ -1910,115 +2332,117 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>86</v>
+        <v>246</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E74" s="12"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>86</v>
+        <v>247</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>86</v>
+        <v>248</v>
       </c>
       <c r="B76" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="12"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="12"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C77" s="1" t="s">
+      <c r="D77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="12"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="12"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="D78" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E78" s="12"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>86</v>
+        <v>251</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E79" s="12"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>86</v>
+        <v>252</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E80" s="12"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="B81" s="7" t="s">
         <v>8</v>
       </c>
@@ -2036,20 +2460,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="56.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -2066,18 +2490,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -2088,15 +2512,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -2105,12 +2529,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -2119,12 +2543,12 @@
         <v>9</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>5</v>
@@ -2137,72 +2561,74 @@
       </c>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -2210,18 +2636,18 @@
       <c r="D11" s="1"/>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>3</v>
@@ -2232,15 +2658,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
@@ -2249,9 +2675,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>5</v>
@@ -2264,15 +2690,15 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
@@ -2281,87 +2707,89 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B17" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="B22" s="16" t="s">
         <v>8</v>
       </c>
@@ -2369,18 +2797,18 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>3</v>
@@ -2391,15 +2819,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>9</v>
@@ -2408,9 +2836,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>5</v>
@@ -2423,15 +2851,15 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>9</v>
@@ -2440,45 +2868,45 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="B28" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>9</v>
@@ -2487,452 +2915,452 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="B36" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="B39" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="B40" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="B42" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
       <c r="B48" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="B51" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>113</v>
+        <v>156</v>
       </c>
       <c r="B54" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="B57" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>9</v>
@@ -2941,38 +3369,40 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="B59" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D60" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="B61" s="16" t="s">
         <v>8</v>
       </c>
@@ -2980,18 +3410,18 @@
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B62" s="17"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="B63" s="16" t="s">
         <v>3</v>
@@ -3002,15 +3432,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>115</v>
+        <v>165</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>9</v>
@@ -3019,39 +3449,39 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>115</v>
+        <v>166</v>
       </c>
       <c r="B65" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B66" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="D66" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>115</v>
+        <v>168</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>5</v>
@@ -3064,15 +3494,15 @@
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>115</v>
+        <v>169</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>9</v>
@@ -3081,9 +3511,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="B69" s="16" t="s">
         <v>5</v>
@@ -3096,32 +3526,32 @@
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>115</v>
+        <v>171</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>115</v>
+        <v>172</v>
       </c>
       <c r="B71" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>9</v>
@@ -3130,9 +3560,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>115</v>
+        <v>173</v>
       </c>
       <c r="B72" s="16" t="s">
         <v>5</v>
@@ -3145,43 +3575,43 @@
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>115</v>
+        <v>176</v>
       </c>
       <c r="B75" s="16" t="s">
         <v>5</v>
@@ -3194,15 +3624,15 @@
       </c>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>9</v>
@@ -3211,8 +3641,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="B77" s="16" t="s">
         <v>8</v>
       </c>

</xml_diff>